<commit_message>
-updated sch and brd, added pdf files
</commit_message>
<xml_diff>
--- a/Doku/Stromwandler_Kennlinie_v2.xlsx
+++ b/Doku/Stromwandler_Kennlinie_v2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Dropbox\Projekte\Leistungsmessung\Doku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Roman\Dropbox\Projekte\Leistungsmessung\Breakout_Board_A1\Doku\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Strom Shunt primär</t>
   </si>
@@ -63,17 +63,53 @@
   </si>
   <si>
     <t>Verältnis Widerstände</t>
+  </si>
+  <si>
+    <t>Strom sekundär in mA RMS</t>
+  </si>
+  <si>
+    <t>Spannung sekundär in mA RMS</t>
+  </si>
+  <si>
+    <t>Messung Kanal 1</t>
+  </si>
+  <si>
+    <t>Messung Kanal 2</t>
+  </si>
+  <si>
+    <t>Messung Kanal 3</t>
+  </si>
+  <si>
+    <t>Messung Kanal 4</t>
+  </si>
+  <si>
+    <t>Mittelwert</t>
+  </si>
+  <si>
+    <t>Abweichung</t>
+  </si>
+  <si>
+    <t>Abweichung in %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,9 +137,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -360,11 +400,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="243304736"/>
-        <c:axId val="244526512"/>
+        <c:axId val="79558064"/>
+        <c:axId val="400991048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="243304736"/>
+        <c:axId val="79558064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,12 +461,12 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="244526512"/>
+        <c:crossAx val="400991048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="244526512"/>
+        <c:axId val="400991048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,7 +523,7 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243304736"/>
+        <c:crossAx val="79558064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1386,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L20"/>
+  <dimension ref="B1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,15 +1439,17 @@
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -1420,8 +1462,24 @@
       <c r="E1">
         <v>4.7</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -1434,8 +1492,32 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0.1</v>
       </c>
@@ -1450,8 +1532,14 @@
         <f>D3/$E$1</f>
         <v>0.68297872340425525</v>
       </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>50.3</v>
+      </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>0.2</v>
       </c>
@@ -1466,8 +1554,14 @@
         <f t="shared" ref="E4:E20" si="1">D4/$E$1</f>
         <v>1.3595744680851063</v>
       </c>
+      <c r="G4">
+        <v>11</v>
+      </c>
+      <c r="H4">
+        <v>55.6</v>
+      </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>0.3</v>
       </c>
@@ -1482,8 +1576,14 @@
         <f t="shared" si="1"/>
         <v>2.0446808510638297</v>
       </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>76.599999999999994</v>
+      </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0.4</v>
       </c>
@@ -1498,8 +1598,32 @@
         <f t="shared" si="1"/>
         <v>2.7234042553191489</v>
       </c>
+      <c r="G6">
+        <v>80</v>
+      </c>
+      <c r="H6">
+        <v>419</v>
+      </c>
+      <c r="I6">
+        <v>80</v>
+      </c>
+      <c r="J6">
+        <v>422</v>
+      </c>
+      <c r="K6">
+        <v>80</v>
+      </c>
+      <c r="L6">
+        <v>419.2</v>
+      </c>
+      <c r="M6">
+        <v>80</v>
+      </c>
+      <c r="N6">
+        <v>420.2</v>
+      </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>0.5</v>
       </c>
@@ -1514,8 +1638,39 @@
         <f t="shared" si="1"/>
         <v>3.4042553191489362</v>
       </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="3">
+        <f>((H6-$F$8)/$F$8)*100</f>
+        <v>-0.26184241847179779</v>
+      </c>
+      <c r="I7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="3">
+        <f>((J6-$F$8)/$F$8)*100</f>
+        <v>0.45227326826945424</v>
+      </c>
+      <c r="K7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="3">
+        <f>((L6-$F$8)/$F$8)*100</f>
+        <v>-0.21423470602238373</v>
+      </c>
+      <c r="M7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="3">
+        <f>((N6-$F$8)/$F$8)*100</f>
+        <v>2.3803856224700281E-2</v>
+      </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.6</v>
       </c>
@@ -1530,8 +1685,12 @@
         <f t="shared" si="1"/>
         <v>4.0872340425531917</v>
       </c>
+      <c r="F8">
+        <f>AVERAGE(H6,J6,L6,N6)</f>
+        <v>420.1</v>
+      </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.7</v>
       </c>
@@ -1547,7 +1706,7 @@
         <v>4.7659574468085104</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.8</v>
       </c>
@@ -1563,7 +1722,7 @@
         <v>5.451063829787234</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.9</v>
       </c>
@@ -1579,7 +1738,7 @@
         <v>6.1319148936170214</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1</v>
       </c>
@@ -1595,7 +1754,7 @@
         <v>6.8106382978723401</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>1.25</v>
       </c>
@@ -1611,7 +1770,7 @@
         <v>8.5106382978723403</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>1.5</v>
       </c>
@@ -1627,7 +1786,7 @@
         <v>10.22127659574468</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>1.75</v>
       </c>
@@ -1643,7 +1802,7 @@
         <v>11.925531914893616</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2</v>
       </c>
@@ -1744,34 +1903,41 @@
         <v>20.436170212765955</v>
       </c>
       <c r="F20">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G20">
         <f>F20*SQRT(2)</f>
-        <v>35.355339059327378</v>
+        <v>49.497474683058329</v>
       </c>
       <c r="H20">
         <f xml:space="preserve"> (E20/C20)*G20</f>
-        <v>80.280858549607416</v>
+        <v>112.39320196945039</v>
       </c>
       <c r="I20">
         <f>H20*$E$1</f>
-        <v>377.32003518315486</v>
+        <v>528.24804925641683</v>
       </c>
       <c r="J20">
         <v>500</v>
       </c>
       <c r="K20">
         <f>J20/I20</f>
-        <v>1.32513504022466</v>
+        <v>0.94652502873189992</v>
       </c>
       <c r="L20">
         <f>K20-1</f>
-        <v>0.32513504022466</v>
+        <v>-5.347497126810008E-2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>